<commit_message>
exp_0407-2031: CDN branch, add relu, real 9 blocks captions
add relu to the CDN mapping linear layer.
In the previous experiments, I mistakenly set the captions number to 4. This time, I correct it.
</commit_message>
<xml_diff>
--- a/data_record.xlsx
+++ b/data_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANewspace\code\smallcap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FD96AB-A879-4952-9922-255C31A0BECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D408715-4A14-4F14-95A7-37567C58BFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15345" xr2:uid="{6D404BE6-E033-4B83-9E31-F2AE59ABBCB5}"/>
+    <workbookView xWindow="7920" yWindow="4695" windowWidth="21600" windowHeight="12645" xr2:uid="{6D404BE6-E033-4B83-9E31-F2AE59ABBCB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Bleu_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,6 +128,14 @@
   </si>
   <si>
     <t>20轮 原始retrieve cap和CDN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格 10轮 CDN，CDN映射层修改，caps数增加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp0407-2031 22140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC12FFEF-9437-4CF7-A837-3D334D1775B7}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.625" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -824,6 +832,44 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>73.569999999999993</v>
+      </c>
+      <c r="C11" s="1">
+        <v>57.13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43.37</v>
+      </c>
+      <c r="E11" s="1">
+        <v>32.74</v>
+      </c>
+      <c r="F11" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="G11" s="1">
+        <v>54.23</v>
+      </c>
+      <c r="H11" s="1">
+        <v>104.77</v>
+      </c>
+      <c r="I11" s="1">
+        <v>18.89</v>
+      </c>
+      <c r="J11" s="1">
+        <v>54.37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
exp_0410-2134: use long sentence as caps
10 epochs, CDN branchs, 9 sentences as caps, bs:128, encoder input length:293

use xmodal-ctx's ctx's retrieve_caps_v2.py to retrieve caps
1. retrieve_caps_v2.py
2. merge_retrieved.py
</commit_message>
<xml_diff>
--- a/data_record.xlsx
+++ b/data_record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANewspace\code\smallcap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D408715-4A14-4F14-95A7-37567C58BFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548BB97-C2DB-4D29-83E6-F82D5DA39817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="4695" windowWidth="21600" windowHeight="12645" xr2:uid="{6D404BE6-E033-4B83-9E31-F2AE59ABBCB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{6D404BE6-E033-4B83-9E31-F2AE59ABBCB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Bleu_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,15 +127,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20轮 原始retrieve cap和CDN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9格 10轮 CDN，CDN映射层修改，caps数增加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exp0407-2031 22140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格 10轮 CDN，CDN映射层修改，caps数为9，以上的caps都是4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_0410-2134/checkpoint-44280</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格 10轮 CDN，映射层一样，caps为9个句子，bs为128，以上的bs都是256，由于句子过长，encoder的输入文本长度为293，而以上的输入文本长度为143</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -508,14 +512,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC12FFEF-9437-4CF7-A837-3D334D1775B7}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.5" customWidth="1"/>
+    <col min="1" max="1" width="17.25" customWidth="1"/>
     <col min="2" max="10" width="9" style="1"/>
+    <col min="12" max="12" width="49.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -551,9 +556,6 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" s="1">
         <v>32.15</v>
       </c>
@@ -566,11 +568,11 @@
       <c r="I2" s="1">
         <v>20.12</v>
       </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
       <c r="B3" s="1">
         <v>75.099999999999994</v>
       </c>
@@ -601,10 +603,13 @@
       <c r="K3" t="s">
         <v>14</v>
       </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>74.92</v>
@@ -637,12 +642,12 @@
         <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
         <v>75.31</v>
@@ -675,12 +680,12 @@
         <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>75.2</v>
@@ -713,13 +718,10 @@
         <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
       <c r="B7" s="1">
         <v>72.400000000000006</v>
       </c>
@@ -750,10 +752,13 @@
       <c r="K7" t="s">
         <v>17</v>
       </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>73.03</v>
@@ -786,12 +791,12 @@
         <v>17</v>
       </c>
       <c r="L8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>76.25</v>
@@ -824,50 +829,83 @@
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
+      <c r="B10" s="1">
+        <v>73.569999999999993</v>
+      </c>
+      <c r="C10" s="1">
+        <v>57.13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43.37</v>
+      </c>
+      <c r="E10" s="1">
+        <v>32.74</v>
+      </c>
+      <c r="F10" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="G10" s="1">
+        <v>54.23</v>
+      </c>
+      <c r="H10" s="1">
+        <v>104.77</v>
+      </c>
+      <c r="I10" s="1">
+        <v>18.89</v>
+      </c>
+      <c r="J10" s="1">
+        <v>54.37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
-        <v>73.569999999999993</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="C11" s="1">
-        <v>57.13</v>
+        <v>52.17</v>
       </c>
       <c r="D11" s="1">
-        <v>43.37</v>
+        <v>38.729999999999997</v>
       </c>
       <c r="E11" s="1">
-        <v>32.74</v>
+        <v>28.7</v>
       </c>
       <c r="F11" s="1">
-        <v>25.7</v>
+        <v>25.12</v>
       </c>
       <c r="G11" s="1">
-        <v>54.23</v>
+        <v>51.89</v>
       </c>
       <c r="H11" s="1">
-        <v>104.77</v>
+        <v>95.31</v>
       </c>
       <c r="I11" s="1">
-        <v>18.89</v>
+        <v>18.37</v>
       </c>
       <c r="J11" s="1">
-        <v>54.37</v>
+        <v>53.2</v>
       </c>
       <c r="K11" t="s">
         <v>17</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exp_0412-1710: caps: two sentence for one images
</commit_message>
<xml_diff>
--- a/data_record.xlsx
+++ b/data_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANewspace\code\smallcap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9548BB97-C2DB-4D29-83E6-F82D5DA39817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B24D0-299B-417E-BD88-1ADE3971C75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{6D404BE6-E033-4B83-9E31-F2AE59ABBCB5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Bleu_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,15 +131,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9格 10轮 CDN，CDN映射层修改，caps数为9，以上的caps都是4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exp_0410-2134/checkpoint-44280</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9格 10轮 CDN，映射层一样，caps为9个句子，bs为128，以上的bs都是256，由于句子过长，encoder的输入文本长度为293，而以上的输入文本长度为143</t>
+    <t>exp_0411-2200/checkpoint-44280</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caps为4个block的句子，其他和以上一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格 10轮 CDN，映射层一样，caps为9个block句子，bs为128，以上的bs都是256，由于句子过长，encoder的输入文本长度为293，而以上的输入文本长度为143</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9格 10轮 CDN，CDN映射层修改，caps数为9block句子，以上的caps都是4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caps为整张图片检索的2个句子，其他一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp_0412-1710/checkpoint-22140</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC12FFEF-9437-4CF7-A837-3D334D1775B7}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -867,12 +883,12 @@
         <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <v>69.099999999999994</v>
@@ -905,7 +921,83 @@
         <v>17</v>
       </c>
       <c r="L11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>71.05</v>
+      </c>
+      <c r="C12" s="1">
+        <v>54.19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>40.53</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30.29</v>
+      </c>
+      <c r="F12" s="1">
+        <v>25.15</v>
+      </c>
+      <c r="G12" s="1">
+        <v>52.55</v>
+      </c>
+      <c r="H12" s="1">
+        <v>98.48</v>
+      </c>
+      <c r="I12" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <v>53.49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="C13" s="1">
+        <v>58.99</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44.99</v>
+      </c>
+      <c r="E13" s="1">
+        <v>34.14</v>
+      </c>
+      <c r="F13" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>55.33</v>
+      </c>
+      <c r="H13" s="1">
+        <v>111.26</v>
+      </c>
+      <c r="I13" s="1">
+        <v>19.87</v>
+      </c>
+      <c r="J13" s="1">
+        <v>55.69</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>